<commit_message>
Updated exercise 1a and 1b
</commit_message>
<xml_diff>
--- a/1_SRE/Part 2/Python for Project Work SRE_Part 2/ERS/ERS_Means/SA_el_hor1_mean.xlsx
+++ b/1_SRE/Part 2/Python for Project Work SRE_Part 2/ERS/ERS_Means/SA_el_hor1_mean.xlsx
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3.3354</v>
+        <v>4.66956</v>
       </c>
     </row>
     <row r="3">
@@ -469,7 +469,7 @@
         <v>50</v>
       </c>
       <c r="C3" t="n">
-        <v>3.441841581627982</v>
+        <v>4.766141795996357</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="n">
-        <v>3.903553450777387</v>
+        <v>5.392781649101257</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +491,7 @@
         <v>16.66666666666667</v>
       </c>
       <c r="C5" t="n">
-        <v>5.56303150191115</v>
+        <v>6.552779326069812</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         <v>12.5</v>
       </c>
       <c r="C6" t="n">
-        <v>6.776923367242692</v>
+        <v>7.779899703025304</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>6.876771366917366</v>
+        <v>9.073270696048676</v>
       </c>
     </row>
     <row r="8">
@@ -524,7 +524,7 @@
         <v>8.333333333333334</v>
       </c>
       <c r="C8" t="n">
-        <v>6.257724489141485</v>
+        <v>9.570853389821844</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         <v>7.142857142857142</v>
       </c>
       <c r="C9" t="n">
-        <v>6.471003947056222</v>
+        <v>10.04780081710842</v>
       </c>
     </row>
     <row r="10">
@@ -546,7 +546,7 @@
         <v>6.25</v>
       </c>
       <c r="C10" t="n">
-        <v>6.783065044700275</v>
+        <v>11.5717557036255</v>
       </c>
     </row>
     <row r="11">
@@ -557,7 +557,7 @@
         <v>5.555555555555555</v>
       </c>
       <c r="C11" t="n">
-        <v>7.777361791916722</v>
+        <v>11.24022259756596</v>
       </c>
     </row>
     <row r="12">
@@ -568,7 +568,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>7.301680667119079</v>
+        <v>11.1607849614282</v>
       </c>
     </row>
     <row r="13">
@@ -579,7 +579,7 @@
         <v>4.545454545454546</v>
       </c>
       <c r="C13" t="n">
-        <v>6.987378945232952</v>
+        <v>10.86783063463396</v>
       </c>
     </row>
     <row r="14">
@@ -590,7 +590,7 @@
         <v>4.166666666666667</v>
       </c>
       <c r="C14" t="n">
-        <v>7.450303777724026</v>
+        <v>11.72702705927065</v>
       </c>
     </row>
     <row r="15">
@@ -601,7 +601,7 @@
         <v>3.846153846153846</v>
       </c>
       <c r="C15" t="n">
-        <v>7.295081594999925</v>
+        <v>12.19573478395733</v>
       </c>
     </row>
     <row r="16">
@@ -612,7 +612,7 @@
         <v>3.571428571428571</v>
       </c>
       <c r="C16" t="n">
-        <v>6.539498848216674</v>
+        <v>11.35521654245341</v>
       </c>
     </row>
     <row r="17">
@@ -623,7 +623,7 @@
         <v>3.333333333333333</v>
       </c>
       <c r="C17" t="n">
-        <v>6.037294311148369</v>
+        <v>10.50588888604132</v>
       </c>
     </row>
     <row r="18">
@@ -634,7 +634,7 @@
         <v>3.125</v>
       </c>
       <c r="C18" t="n">
-        <v>5.950520511162642</v>
+        <v>10.05327278842635</v>
       </c>
     </row>
     <row r="19">
@@ -645,7 +645,7 @@
         <v>2.941176470588235</v>
       </c>
       <c r="C19" t="n">
-        <v>5.600310643412475</v>
+        <v>9.340367684209077</v>
       </c>
     </row>
     <row r="20">
@@ -656,7 +656,7 @@
         <v>2.777777777777778</v>
       </c>
       <c r="C20" t="n">
-        <v>5.256888793147048</v>
+        <v>8.719436360908738</v>
       </c>
     </row>
     <row r="21">
@@ -667,7 +667,7 @@
         <v>2.631578947368421</v>
       </c>
       <c r="C21" t="n">
-        <v>4.93418014730595</v>
+        <v>8.368288049649799</v>
       </c>
     </row>
     <row r="22">
@@ -678,7 +678,7 @@
         <v>2.5</v>
       </c>
       <c r="C22" t="n">
-        <v>4.898781491011488</v>
+        <v>8.249444315576609</v>
       </c>
     </row>
     <row r="23">
@@ -689,7 +689,7 @@
         <v>2.380952380952381</v>
       </c>
       <c r="C23" t="n">
-        <v>4.68612538544807</v>
+        <v>7.836836558644321</v>
       </c>
     </row>
     <row r="24">
@@ -700,7 +700,7 @@
         <v>2.272727272727273</v>
       </c>
       <c r="C24" t="n">
-        <v>4.657962474721367</v>
+        <v>7.760494383140789</v>
       </c>
     </row>
     <row r="25">
@@ -711,7 +711,7 @@
         <v>2.173913043478261</v>
       </c>
       <c r="C25" t="n">
-        <v>4.592136263263883</v>
+        <v>7.571052927547834</v>
       </c>
     </row>
     <row r="26">
@@ -722,7 +722,7 @@
         <v>2.083333333333333</v>
       </c>
       <c r="C26" t="n">
-        <v>4.117699386077306</v>
+        <v>6.844176794251674</v>
       </c>
     </row>
     <row r="27">
@@ -733,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>3.641446470706458</v>
+        <v>6.08620179636113</v>
       </c>
     </row>
     <row r="28">
@@ -744,7 +744,7 @@
         <v>1.923076923076923</v>
       </c>
       <c r="C28" t="n">
-        <v>3.316008223444556</v>
+        <v>5.488745382180859</v>
       </c>
     </row>
     <row r="29">
@@ -755,7 +755,7 @@
         <v>1.851851851851852</v>
       </c>
       <c r="C29" t="n">
-        <v>2.898634836187417</v>
+        <v>4.811578810102412</v>
       </c>
     </row>
     <row r="30">
@@ -766,7 +766,7 @@
         <v>1.785714285714286</v>
       </c>
       <c r="C30" t="n">
-        <v>2.468151485965811</v>
+        <v>4.123290183582755</v>
       </c>
     </row>
     <row r="31">
@@ -777,7 +777,7 @@
         <v>1.724137931034483</v>
       </c>
       <c r="C31" t="n">
-        <v>2.215486068233788</v>
+        <v>3.693788667114045</v>
       </c>
     </row>
     <row r="32">
@@ -788,7 +788,7 @@
         <v>1.666666666666667</v>
       </c>
       <c r="C32" t="n">
-        <v>2.042807946458995</v>
+        <v>3.415491510808521</v>
       </c>
     </row>
     <row r="33">
@@ -799,7 +799,7 @@
         <v>1.612903225806452</v>
       </c>
       <c r="C33" t="n">
-        <v>1.871851212084287</v>
+        <v>3.177617791410474</v>
       </c>
     </row>
     <row r="34">
@@ -810,7 +810,7 @@
         <v>1.5625</v>
       </c>
       <c r="C34" t="n">
-        <v>1.721935106997655</v>
+        <v>2.951776323750849</v>
       </c>
     </row>
     <row r="35">
@@ -821,7 +821,7 @@
         <v>1.515151515151515</v>
       </c>
       <c r="C35" t="n">
-        <v>1.579913524383497</v>
+        <v>2.753753328190655</v>
       </c>
     </row>
     <row r="36">
@@ -832,7 +832,7 @@
         <v>1.470588235294118</v>
       </c>
       <c r="C36" t="n">
-        <v>1.45560522144947</v>
+        <v>2.585504775377692</v>
       </c>
     </row>
     <row r="37">
@@ -843,7 +843,7 @@
         <v>1.428571428571428</v>
       </c>
       <c r="C37" t="n">
-        <v>1.353310474366461</v>
+        <v>2.422294926229111</v>
       </c>
     </row>
     <row r="38">
@@ -854,7 +854,7 @@
         <v>1.388888888888889</v>
       </c>
       <c r="C38" t="n">
-        <v>1.264583348107427</v>
+        <v>2.262306321406899</v>
       </c>
     </row>
     <row r="39">
@@ -865,7 +865,7 @@
         <v>1.351351351351351</v>
       </c>
       <c r="C39" t="n">
-        <v>1.176060670555429</v>
+        <v>2.141006469405349</v>
       </c>
     </row>
     <row r="40">
@@ -876,7 +876,7 @@
         <v>1.315789473684211</v>
       </c>
       <c r="C40" t="n">
-        <v>1.091890174026715</v>
+        <v>2.02769333245773</v>
       </c>
     </row>
     <row r="41">
@@ -887,7 +887,7 @@
         <v>1.282051282051282</v>
       </c>
       <c r="C41" t="n">
-        <v>1.018534753643135</v>
+        <v>1.920268642280728</v>
       </c>
     </row>
     <row r="42">
@@ -898,7 +898,7 @@
         <v>1.25</v>
       </c>
       <c r="C42" t="n">
-        <v>0.9507504356301664</v>
+        <v>1.814041899940717</v>
       </c>
     </row>
     <row r="43">
@@ -909,7 +909,7 @@
         <v>1.219512195121951</v>
       </c>
       <c r="C43" t="n">
-        <v>0.906251465751341</v>
+        <v>1.737948252700595</v>
       </c>
     </row>
     <row r="44">
@@ -920,7 +920,7 @@
         <v>1.19047619047619</v>
       </c>
       <c r="C44" t="n">
-        <v>0.8604229655793911</v>
+        <v>1.655008381247813</v>
       </c>
     </row>
     <row r="45">
@@ -931,7 +931,7 @@
         <v>1.162790697674419</v>
       </c>
       <c r="C45" t="n">
-        <v>0.8147239484168769</v>
+        <v>1.568708293016981</v>
       </c>
     </row>
     <row r="46">
@@ -942,7 +942,7 @@
         <v>1.136363636363636</v>
       </c>
       <c r="C46" t="n">
-        <v>0.7658693821492178</v>
+        <v>1.490316852621896</v>
       </c>
     </row>
     <row r="47">
@@ -953,7 +953,7 @@
         <v>1.111111111111111</v>
       </c>
       <c r="C47" t="n">
-        <v>0.7220430534279165</v>
+        <v>1.416867445675534</v>
       </c>
     </row>
     <row r="48">
@@ -964,7 +964,7 @@
         <v>1.08695652173913</v>
       </c>
       <c r="C48" t="n">
-        <v>0.6904338128667262</v>
+        <v>1.356013674823543</v>
       </c>
     </row>
     <row r="49">
@@ -975,7 +975,7 @@
         <v>1.063829787234043</v>
       </c>
       <c r="C49" t="n">
-        <v>0.6678155331303863</v>
+        <v>1.303502772776963</v>
       </c>
     </row>
     <row r="50">
@@ -986,7 +986,7 @@
         <v>1.041666666666667</v>
       </c>
       <c r="C50" t="n">
-        <v>0.6316993240030895</v>
+        <v>1.231196683296316</v>
       </c>
     </row>
     <row r="51">
@@ -997,7 +997,7 @@
         <v>1.020408163265306</v>
       </c>
       <c r="C51" t="n">
-        <v>0.6055826676896306</v>
+        <v>1.171214689636681</v>
       </c>
     </row>
     <row r="52">
@@ -1008,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>0.5800973887795444</v>
+        <v>1.10904981380708</v>
       </c>
     </row>
     <row r="53">
@@ -1019,7 +1019,7 @@
         <v>0.9803921568627451</v>
       </c>
       <c r="C53" t="n">
-        <v>0.5538859806358433</v>
+        <v>1.045999865226658</v>
       </c>
     </row>
     <row r="54">
@@ -1030,7 +1030,7 @@
         <v>0.9615384615384615</v>
       </c>
       <c r="C54" t="n">
-        <v>0.5334589325018165</v>
+        <v>0.9930765200425662</v>
       </c>
     </row>
     <row r="55">
@@ -1041,7 +1041,7 @@
         <v>0.9433962264150942</v>
       </c>
       <c r="C55" t="n">
-        <v>0.5144042598768946</v>
+        <v>0.9532668239990715</v>
       </c>
     </row>
     <row r="56">
@@ -1052,7 +1052,7 @@
         <v>0.9259259259259258</v>
       </c>
       <c r="C56" t="n">
-        <v>0.4949449985915196</v>
+        <v>0.9151148451495736</v>
       </c>
     </row>
     <row r="57">
@@ -1063,7 +1063,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="C57" t="n">
-        <v>0.4754431217840285</v>
+        <v>0.8779573180736373</v>
       </c>
     </row>
     <row r="58">
@@ -1074,7 +1074,7 @@
         <v>0.8928571428571428</v>
       </c>
       <c r="C58" t="n">
-        <v>0.4564065220709716</v>
+        <v>0.8417124212556201</v>
       </c>
     </row>
     <row r="59">
@@ -1085,7 +1085,7 @@
         <v>0.8771929824561403</v>
       </c>
       <c r="C59" t="n">
-        <v>0.4426298806711381</v>
+        <v>0.8127853278065922</v>
       </c>
     </row>
     <row r="60">
@@ -1096,7 +1096,7 @@
         <v>0.8620689655172414</v>
       </c>
       <c r="C60" t="n">
-        <v>0.4335443855341153</v>
+        <v>0.7892721916103843</v>
       </c>
     </row>
     <row r="61">
@@ -1107,7 +1107,7 @@
         <v>0.8474576271186441</v>
       </c>
       <c r="C61" t="n">
-        <v>0.4204078926416271</v>
+        <v>0.759815845430144</v>
       </c>
     </row>
     <row r="62">
@@ -1118,7 +1118,7 @@
         <v>0.8333333333333334</v>
       </c>
       <c r="C62" t="n">
-        <v>0.4039206734211298</v>
+        <v>0.7255603595029965</v>
       </c>
     </row>
     <row r="63">
@@ -1129,7 +1129,7 @@
         <v>0.819672131147541</v>
       </c>
       <c r="C63" t="n">
-        <v>0.3853248654360737</v>
+        <v>0.6919675700174578</v>
       </c>
     </row>
     <row r="64">
@@ -1140,7 +1140,7 @@
         <v>0.8064516129032259</v>
       </c>
       <c r="C64" t="n">
-        <v>0.3678091739290985</v>
+        <v>0.6599504838410785</v>
       </c>
     </row>
     <row r="65">
@@ -1151,7 +1151,7 @@
         <v>0.7936507936507936</v>
       </c>
       <c r="C65" t="n">
-        <v>0.3568638707013626</v>
+        <v>0.6372250542722157</v>
       </c>
     </row>
     <row r="66">
@@ -1162,7 +1162,7 @@
         <v>0.78125</v>
       </c>
       <c r="C66" t="n">
-        <v>0.3465072551374878</v>
+        <v>0.6155661938971689</v>
       </c>
     </row>
     <row r="67">
@@ -1173,7 +1173,7 @@
         <v>0.7692307692307692</v>
       </c>
       <c r="C67" t="n">
-        <v>0.3366366977544095</v>
+        <v>0.5948984855203692</v>
       </c>
     </row>
     <row r="68">
@@ -1184,7 +1184,7 @@
         <v>0.7575757575757576</v>
       </c>
       <c r="C68" t="n">
-        <v>0.3271888218761054</v>
+        <v>0.5751636886354589</v>
       </c>
     </row>
     <row r="69">
@@ -1195,7 +1195,7 @@
         <v>0.7462686567164178</v>
       </c>
       <c r="C69" t="n">
-        <v>0.3181123392486734</v>
+        <v>0.5563100496724814</v>
       </c>
     </row>
     <row r="70">
@@ -1206,7 +1206,7 @@
         <v>0.7352941176470588</v>
       </c>
       <c r="C70" t="n">
-        <v>0.3095044327991399</v>
+        <v>0.538292810144415</v>
       </c>
     </row>
     <row r="71">
@@ -1217,7 +1217,7 @@
         <v>0.7246376811594202</v>
       </c>
       <c r="C71" t="n">
-        <v>0.3013232027204476</v>
+        <v>0.5210735714358179</v>
       </c>
     </row>
     <row r="72">
@@ -1228,7 +1228,7 @@
         <v>0.7142857142857142</v>
       </c>
       <c r="C72" t="n">
-        <v>0.2934408699383347</v>
+        <v>0.5046671435858306</v>
       </c>
     </row>
     <row r="73">
@@ -1239,7 +1239,7 @@
         <v>0.7042253521126761</v>
       </c>
       <c r="C73" t="n">
-        <v>0.2858238999133893</v>
+        <v>0.4898114525374984</v>
       </c>
     </row>
     <row r="74">
@@ -1250,7 +1250,7 @@
         <v>0.6944444444444444</v>
       </c>
       <c r="C74" t="n">
-        <v>0.2784485800180886</v>
+        <v>0.4755692575510804</v>
       </c>
     </row>
     <row r="75">
@@ -1261,7 +1261,7 @@
         <v>0.684931506849315</v>
       </c>
       <c r="C75" t="n">
-        <v>0.2717892384885744</v>
+        <v>0.4618922562271285</v>
       </c>
     </row>
     <row r="76">
@@ -1272,7 +1272,7 @@
         <v>0.6756756756756757</v>
       </c>
       <c r="C76" t="n">
-        <v>0.2654707506433106</v>
+        <v>0.4488005646763696</v>
       </c>
     </row>
     <row r="77">
@@ -1283,7 +1283,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="C77" t="n">
-        <v>0.2593127255866157</v>
+        <v>0.4362423479449425</v>
       </c>
     </row>
     <row r="78">
@@ -1294,7 +1294,7 @@
         <v>0.6578947368421053</v>
       </c>
       <c r="C78" t="n">
-        <v>0.2533113238366764</v>
+        <v>0.4242221081455671</v>
       </c>
     </row>
     <row r="79">
@@ -1305,7 +1305,7 @@
         <v>0.6493506493506493</v>
       </c>
       <c r="C79" t="n">
-        <v>0.2474690090373402</v>
+        <v>0.4127070937267562</v>
       </c>
     </row>
     <row r="80">
@@ -1316,7 +1316,7 @@
         <v>0.641025641025641</v>
       </c>
       <c r="C80" t="n">
-        <v>0.2417890865561336</v>
+        <v>0.4017240984246875</v>
       </c>
     </row>
     <row r="81">
@@ -1327,7 +1327,7 @@
         <v>0.6329113924050632</v>
       </c>
       <c r="C81" t="n">
-        <v>0.2362627218993807</v>
+        <v>0.3912048358724734</v>
       </c>
     </row>
     <row r="82">
@@ -1338,7 +1338,7 @@
         <v>0.625</v>
       </c>
       <c r="C82" t="n">
-        <v>0.2308877974290287</v>
+        <v>0.381102175517246</v>
       </c>
     </row>
     <row r="83">
@@ -1349,7 +1349,7 @@
         <v>0.6172839506172839</v>
       </c>
       <c r="C83" t="n">
-        <v>0.225618537337639</v>
+        <v>0.3713824872628739</v>
       </c>
     </row>
     <row r="84">
@@ -1360,7 +1360,7 @@
         <v>0.6097560975609756</v>
       </c>
       <c r="C84" t="n">
-        <v>0.220411631331432</v>
+        <v>0.361998479516015</v>
       </c>
     </row>
     <row r="85">
@@ -1371,7 +1371,7 @@
         <v>0.6024096385542168</v>
       </c>
       <c r="C85" t="n">
-        <v>0.2152361422374453</v>
+        <v>0.3529496509803635</v>
       </c>
     </row>
     <row r="86">
@@ -1382,7 +1382,7 @@
         <v>0.5952380952380952</v>
       </c>
       <c r="C86" t="n">
-        <v>0.2100665221668176</v>
+        <v>0.3441984400765128</v>
       </c>
     </row>
     <row r="87">
@@ -1393,7 +1393,7 @@
         <v>0.5882352941176471</v>
       </c>
       <c r="C87" t="n">
-        <v>0.204867317152544</v>
+        <v>0.3357316126936048</v>
       </c>
     </row>
     <row r="88">
@@ -1404,7 +1404,7 @@
         <v>0.5813953488372093</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1996353907550845</v>
+        <v>0.3275266432029752</v>
       </c>
     </row>
     <row r="89">
@@ -1415,7 +1415,7 @@
         <v>0.5747126436781609</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1943536780915634</v>
+        <v>0.3195827966479705</v>
       </c>
     </row>
     <row r="90">
@@ -1426,7 +1426,7 @@
         <v>0.5681818181818182</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1894342173199151</v>
+        <v>0.3118827986390912</v>
       </c>
     </row>
     <row r="91">
@@ -1437,7 +1437,7 @@
         <v>0.5617977528089888</v>
       </c>
       <c r="C91" t="n">
-        <v>0.184887146666971</v>
+        <v>0.3047564913307952</v>
       </c>
     </row>
     <row r="92">
@@ -1448,7 +1448,7 @@
         <v>0.5555555555555556</v>
       </c>
       <c r="C92" t="n">
-        <v>0.1816879548590982</v>
+        <v>0.2987174632985444</v>
       </c>
     </row>
     <row r="93">
@@ -1459,7 +1459,7 @@
         <v>0.5494505494505494</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1787095595097866</v>
+        <v>0.2927383463611361</v>
       </c>
     </row>
     <row r="94">
@@ -1470,7 +1470,7 @@
         <v>0.5434782608695652</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1756336817465377</v>
+        <v>0.2867933328153012</v>
       </c>
     </row>
     <row r="95">
@@ -1481,7 +1481,7 @@
         <v>0.5376344086021505</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1723516503132926</v>
+        <v>0.2808556403452021</v>
       </c>
     </row>
     <row r="96">
@@ -1492,7 +1492,7 @@
         <v>0.5319148936170213</v>
       </c>
       <c r="C96" t="n">
-        <v>0.1688446295802096</v>
+        <v>0.274917201836946</v>
       </c>
     </row>
     <row r="97">
@@ -1503,7 +1503,7 @@
         <v>0.5263157894736842</v>
       </c>
       <c r="C97" t="n">
-        <v>0.165120533663636</v>
+        <v>0.2689577983320116</v>
       </c>
     </row>
     <row r="98">
@@ -1514,7 +1514,7 @@
         <v>0.5208333333333334</v>
       </c>
       <c r="C98" t="n">
-        <v>0.1615134181040115</v>
+        <v>0.2629721409853242</v>
       </c>
     </row>
     <row r="99">
@@ -1525,7 +1525,7 @@
         <v>0.5154639175257733</v>
       </c>
       <c r="C99" t="n">
-        <v>0.1577993413081958</v>
+        <v>0.2569742136942352</v>
       </c>
     </row>
     <row r="100">
@@ -1536,7 +1536,7 @@
         <v>0.5102040816326531</v>
       </c>
       <c r="C100" t="n">
-        <v>0.1539874689950824</v>
+        <v>0.2513284912726928</v>
       </c>
     </row>
     <row r="101">
@@ -1547,7 +1547,7 @@
         <v>0.5050505050505051</v>
       </c>
       <c r="C101" t="n">
-        <v>0.1500824195784591</v>
+        <v>0.2456699673210433</v>
       </c>
     </row>
     <row r="102">
@@ -1558,7 +1558,7 @@
         <v>0.5</v>
       </c>
       <c r="C102" t="n">
-        <v>0.1461083368209901</v>
+        <v>0.2400111388178086</v>
       </c>
     </row>
     <row r="103">
@@ -1569,7 +1569,7 @@
         <v>0.495049504950495</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1420983028228292</v>
+        <v>0.234371335160068</v>
       </c>
     </row>
     <row r="104">
@@ -1580,7 +1580,7 @@
         <v>0.4901960784313725</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1380757079094657</v>
+        <v>0.2287718368667921</v>
       </c>
     </row>
     <row r="105">
@@ -1591,7 +1591,7 @@
         <v>0.4854368932038835</v>
       </c>
       <c r="C105" t="n">
-        <v>0.1344111237494825</v>
+        <v>0.223721269974414</v>
       </c>
     </row>
     <row r="106">
@@ -1602,7 +1602,7 @@
         <v>0.4807692307692307</v>
       </c>
       <c r="C106" t="n">
-        <v>0.1313064187246471</v>
+        <v>0.2194900306499511</v>
       </c>
     </row>
     <row r="107">
@@ -1613,7 +1613,7 @@
         <v>0.4761904761904762</v>
       </c>
       <c r="C107" t="n">
-        <v>0.1283897877429746</v>
+        <v>0.2155422481332893</v>
       </c>
     </row>
     <row r="108">
@@ -1624,7 +1624,7 @@
         <v>0.4716981132075471</v>
       </c>
       <c r="C108" t="n">
-        <v>0.1266175296556316</v>
+        <v>0.2130466455598652</v>
       </c>
     </row>
     <row r="109">
@@ -1635,7 +1635,7 @@
         <v>0.4672897196261682</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1251899241600316</v>
+        <v>0.2105189687600162</v>
       </c>
     </row>
     <row r="110">
@@ -1646,7 +1646,7 @@
         <v>0.4629629629629629</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1237100576951323</v>
+        <v>0.2079509846979763</v>
       </c>
     </row>
     <row r="111">
@@ -1657,7 +1657,7 @@
         <v>0.4587155963302752</v>
       </c>
       <c r="C111" t="n">
-        <v>0.1221755557251245</v>
+        <v>0.2053376808167146</v>
       </c>
     </row>
     <row r="112">
@@ -1668,7 +1668,7 @@
         <v>0.4545454545454545</v>
       </c>
       <c r="C112" t="n">
-        <v>0.1205857326127883</v>
+        <v>0.2026769209249041</v>
       </c>
     </row>
     <row r="113">
@@ -1679,7 +1679,7 @@
         <v>0.4504504504504504</v>
       </c>
       <c r="C113" t="n">
-        <v>0.1190024707094521</v>
+        <v>0.1999690550349188</v>
       </c>
     </row>
     <row r="114">
@@ -1690,7 +1690,7 @@
         <v>0.4464285714285714</v>
       </c>
       <c r="C114" t="n">
-        <v>0.117493801586035</v>
+        <v>0.1972241429706212</v>
       </c>
     </row>
     <row r="115">
@@ -1701,7 +1701,7 @@
         <v>0.4424778761061947</v>
       </c>
       <c r="C115" t="n">
-        <v>0.1159432561704955</v>
+        <v>0.1944406841373518</v>
       </c>
     </row>
     <row r="116">
@@ -1712,7 +1712,7 @@
         <v>0.4385964912280702</v>
       </c>
       <c r="C116" t="n">
-        <v>0.1143528192229519</v>
+        <v>0.1916215750379462</v>
       </c>
     </row>
     <row r="117">
@@ -1723,7 +1723,7 @@
         <v>0.4347826086956521</v>
       </c>
       <c r="C117" t="n">
-        <v>0.1127303831197807</v>
+        <v>0.1887781465555982</v>
       </c>
     </row>
     <row r="118">
@@ -1734,7 +1734,7 @@
         <v>0.4310344827586207</v>
       </c>
       <c r="C118" t="n">
-        <v>0.1110789062022718</v>
+        <v>0.1859149232496641</v>
       </c>
     </row>
     <row r="119">
@@ -1745,7 +1745,7 @@
         <v>0.4273504273504274</v>
       </c>
       <c r="C119" t="n">
-        <v>0.1094008434984897</v>
+        <v>0.1830357710917334</v>
       </c>
     </row>
     <row r="120">
@@ -1756,7 +1756,7 @@
         <v>0.4237288135593221</v>
       </c>
       <c r="C120" t="n">
-        <v>0.1077010010268036</v>
+        <v>0.1801478459079597</v>
       </c>
     </row>
     <row r="121">
@@ -1767,7 +1767,7 @@
         <v>0.4201680672268908</v>
       </c>
       <c r="C121" t="n">
-        <v>0.1059841275506155</v>
+        <v>0.1772581821504624</v>
       </c>
     </row>
     <row r="122">
@@ -1778,7 +1778,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="C122" t="n">
-        <v>0.104254826107433</v>
+        <v>0.1743735371273296</v>
       </c>
     </row>
     <row r="123">
@@ -1789,7 +1789,7 @@
         <v>0.4132231404958678</v>
       </c>
       <c r="C123" t="n">
-        <v>0.1025206730748832</v>
+        <v>0.1715047332155001</v>
       </c>
     </row>
     <row r="124">
@@ -1800,7 +1800,7 @@
         <v>0.4098360655737705</v>
       </c>
       <c r="C124" t="n">
-        <v>0.1007832797245176</v>
+        <v>0.1686621859759894</v>
       </c>
     </row>
     <row r="125">
@@ -1811,7 +1811,7 @@
         <v>0.4065040650406504</v>
       </c>
       <c r="C125" t="n">
-        <v>0.09904574404914442</v>
+        <v>0.1658698846953454</v>
       </c>
     </row>
     <row r="126">
@@ -1822,7 +1822,7 @@
         <v>0.4032258064516129</v>
       </c>
       <c r="C126" t="n">
-        <v>0.09731162202416115</v>
+        <v>0.1631083025390562</v>
       </c>
     </row>
     <row r="127">
@@ -1833,7 +1833,7 @@
         <v>0.4</v>
       </c>
       <c r="C127" t="n">
-        <v>0.09558504799973221</v>
+        <v>0.1603807006277175</v>
       </c>
     </row>
     <row r="128">
@@ -1844,7 +1844,7 @@
         <v>0.3968253968253968</v>
       </c>
       <c r="C128" t="n">
-        <v>0.0938688711572068</v>
+        <v>0.1576883296320939</v>
       </c>
     </row>
     <row r="129">
@@ -1855,7 +1855,7 @@
         <v>0.3937007874015748</v>
       </c>
       <c r="C129" t="n">
-        <v>0.09216456076882748</v>
+        <v>0.1550327356598127</v>
       </c>
     </row>
     <row r="130">
@@ -1866,7 +1866,7 @@
         <v>0.390625</v>
       </c>
       <c r="C130" t="n">
-        <v>0.09047455383863136</v>
+        <v>0.1524167034784195</v>
       </c>
     </row>
     <row r="131">
@@ -1877,7 +1877,7 @@
         <v>0.3875968992248062</v>
       </c>
       <c r="C131" t="n">
-        <v>0.08880104103162251</v>
+        <v>0.149842567884141</v>
       </c>
     </row>
     <row r="132">
@@ -1888,7 +1888,7 @@
         <v>0.3846153846153846</v>
       </c>
       <c r="C132" t="n">
-        <v>0.08714598747430369</v>
+        <v>0.1473122552687353</v>
       </c>
     </row>
     <row r="133">
@@ -1899,7 +1899,7 @@
         <v>0.3816793893129771</v>
       </c>
       <c r="C133" t="n">
-        <v>0.08551115377505579</v>
+        <v>0.1448330623809952</v>
       </c>
     </row>
     <row r="134">
@@ -1910,7 +1910,7 @@
         <v>0.3787878787878788</v>
       </c>
       <c r="C134" t="n">
-        <v>0.08389811634912533</v>
+        <v>0.142401943067803</v>
       </c>
     </row>
     <row r="135">
@@ -1921,7 +1921,7 @@
         <v>0.3759398496240601</v>
       </c>
       <c r="C135" t="n">
-        <v>0.08230828642503865</v>
+        <v>0.1400181857500074</v>
       </c>
     </row>
     <row r="136">
@@ -1932,7 +1932,7 @@
         <v>0.3731343283582089</v>
       </c>
       <c r="C136" t="n">
-        <v>0.08074292731497565</v>
+        <v>0.1376825062813098</v>
       </c>
     </row>
     <row r="137">
@@ -1943,7 +1943,7 @@
         <v>0.3703703703703703</v>
       </c>
       <c r="C137" t="n">
-        <v>0.07920316968848537</v>
+        <v>0.1353954093172164</v>
       </c>
     </row>
     <row r="138">
@@ -1954,7 +1954,7 @@
         <v>0.3676470588235294</v>
       </c>
       <c r="C138" t="n">
-        <v>0.07769002477038268</v>
+        <v>0.1331572190939753</v>
       </c>
     </row>
     <row r="139">
@@ -1965,7 +1965,7 @@
         <v>0.364963503649635</v>
       </c>
       <c r="C139" t="n">
-        <v>0.0762914535117331</v>
+        <v>0.1309702189788994</v>
       </c>
     </row>
     <row r="140">
@@ -1976,7 +1976,7 @@
         <v>0.3623188405797101</v>
       </c>
       <c r="C140" t="n">
-        <v>0.0750297035078196</v>
+        <v>0.128832675287896</v>
       </c>
     </row>
     <row r="141">
@@ -1987,7 +1987,7 @@
         <v>0.3597122302158273</v>
       </c>
       <c r="C141" t="n">
-        <v>0.07406679292098026</v>
+        <v>0.1269794780651069</v>
       </c>
     </row>
     <row r="142">
@@ -1998,7 +1998,7 @@
         <v>0.3571428571428571</v>
       </c>
       <c r="C142" t="n">
-        <v>0.07322517589339701</v>
+        <v>0.1252881651785913</v>
       </c>
     </row>
     <row r="143">
@@ -2009,7 +2009,7 @@
         <v>0.3546099290780142</v>
       </c>
       <c r="C143" t="n">
-        <v>0.072376685530757</v>
+        <v>0.1236305932446499</v>
       </c>
     </row>
     <row r="144">
@@ -2020,7 +2020,7 @@
         <v>0.3521126760563381</v>
       </c>
       <c r="C144" t="n">
-        <v>0.07148948471342188</v>
+        <v>0.1220060297161639</v>
       </c>
     </row>
     <row r="145">
@@ -2031,7 +2031,7 @@
         <v>0.3496503496503497</v>
       </c>
       <c r="C145" t="n">
-        <v>0.07055985999486837</v>
+        <v>0.1204137546483254</v>
       </c>
     </row>
     <row r="146">
@@ -2042,7 +2042,7 @@
         <v>0.3472222222222222</v>
       </c>
       <c r="C146" t="n">
-        <v>0.06961601669616548</v>
+        <v>0.1188530593506415</v>
       </c>
     </row>
     <row r="147">
@@ -2053,7 +2053,7 @@
         <v>0.3448275862068966</v>
       </c>
       <c r="C147" t="n">
-        <v>0.06877268053026479</v>
+        <v>0.1173232454171114</v>
       </c>
     </row>
     <row r="148">
@@ -2064,7 +2064,7 @@
         <v>0.3424657534246575</v>
       </c>
       <c r="C148" t="n">
-        <v>0.06792346714661465</v>
+        <v>0.1158308734825324</v>
       </c>
     </row>
     <row r="149">
@@ -2075,7 +2075,7 @@
         <v>0.3401360544217687</v>
       </c>
       <c r="C149" t="n">
-        <v>0.06706622115532521</v>
+        <v>0.1143712653672209</v>
       </c>
     </row>
     <row r="150">
@@ -2086,7 +2086,7 @@
         <v>0.3378378378378378</v>
       </c>
       <c r="C150" t="n">
-        <v>0.06619946651450329</v>
+        <v>0.1129402216727113</v>
       </c>
     </row>
     <row r="151">
@@ -2097,7 +2097,7 @@
         <v>0.3355704697986577</v>
       </c>
       <c r="C151" t="n">
-        <v>0.06532453770748911</v>
+        <v>0.1115370903417228</v>
       </c>
     </row>
     <row r="152">
@@ -2108,7 +2108,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="C152" t="n">
-        <v>0.06444299295230624</v>
+        <v>0.1101612281355768</v>
       </c>
     </row>
     <row r="153">
@@ -2119,7 +2119,7 @@
         <v>0.3311258278145696</v>
       </c>
       <c r="C153" t="n">
-        <v>0.06355655768276686</v>
+        <v>0.1088120008946374</v>
       </c>
     </row>
     <row r="154">
@@ -2130,7 +2130,7 @@
         <v>0.3289473684210527</v>
       </c>
       <c r="C154" t="n">
-        <v>0.06266707160410714</v>
+        <v>0.1074887838700318</v>
       </c>
     </row>
     <row r="155">
@@ -2141,7 +2141,7 @@
         <v>0.326797385620915</v>
       </c>
       <c r="C155" t="n">
-        <v>0.06177855398298959</v>
+        <v>0.1061909620972257</v>
       </c>
     </row>
     <row r="156">
@@ -2152,7 +2152,7 @@
         <v>0.3246753246753247</v>
       </c>
       <c r="C156" t="n">
-        <v>0.06089087228539717</v>
+        <v>0.1049179307884414</v>
       </c>
     </row>
     <row r="157">
@@ -2163,7 +2163,7 @@
         <v>0.3225806451612903</v>
       </c>
       <c r="C157" t="n">
-        <v>0.06000567972967978</v>
+        <v>0.1036690957303462</v>
       </c>
     </row>
     <row r="158">
@@ -2174,7 +2174,7 @@
         <v>0.3205128205128205</v>
       </c>
       <c r="C158" t="n">
-        <v>0.05916409038975158</v>
+        <v>0.1024472421890088</v>
       </c>
     </row>
     <row r="159">
@@ -2185,7 +2185,7 @@
         <v>0.3184713375796178</v>
       </c>
       <c r="C159" t="n">
-        <v>0.05837708598748986</v>
+        <v>0.1012490966896329</v>
       </c>
     </row>
     <row r="160">
@@ -2196,7 +2196,7 @@
         <v>0.3164556962025316</v>
       </c>
       <c r="C160" t="n">
-        <v>0.05759606580707794</v>
+        <v>0.1000733370683739</v>
       </c>
     </row>
     <row r="161">
@@ -2207,7 +2207,7 @@
         <v>0.3144654088050314</v>
       </c>
       <c r="C161" t="n">
-        <v>0.05688290258236645</v>
+        <v>0.09891941645955091</v>
       </c>
     </row>
     <row r="162">
@@ -2218,7 +2218,7 @@
         <v>0.3125</v>
       </c>
       <c r="C162" t="n">
-        <v>0.05617269512800295</v>
+        <v>0.09778680025389043</v>
       </c>
     </row>
     <row r="163">
@@ -2229,7 +2229,7 @@
         <v>0.3105590062111801</v>
       </c>
       <c r="C163" t="n">
-        <v>0.05545522575935408</v>
+        <v>0.09667496629346521</v>
       </c>
     </row>
     <row r="164">
@@ -2240,7 +2240,7 @@
         <v>0.308641975308642</v>
       </c>
       <c r="C164" t="n">
-        <v>0.05473259125100099</v>
+        <v>0.09558340503388002</v>
       </c>
     </row>
     <row r="165">
@@ -2251,7 +2251,7 @@
         <v>0.3067484662576687</v>
       </c>
       <c r="C165" t="n">
-        <v>0.05400687270163993</v>
+        <v>0.09451161964345181</v>
       </c>
     </row>
     <row r="166">
@@ -2262,7 +2262,7 @@
         <v>0.3048780487804878</v>
       </c>
       <c r="C166" t="n">
-        <v>0.0532800968171616</v>
+        <v>0.09345912606661876</v>
       </c>
     </row>
     <row r="167">
@@ -2273,7 +2273,7 @@
         <v>0.303030303030303</v>
       </c>
       <c r="C167" t="n">
-        <v>0.05265252081814074</v>
+        <v>0.0924254530403565</v>
       </c>
     </row>
     <row r="168">
@@ -2284,7 +2284,7 @@
         <v>0.3012048192771084</v>
       </c>
       <c r="C168" t="n">
-        <v>0.05202641553133701</v>
+        <v>0.0914101420661317</v>
       </c>
     </row>
     <row r="169">
@@ -2295,7 +2295,7 @@
         <v>0.2994011976047904</v>
       </c>
       <c r="C169" t="n">
-        <v>0.05140184204487139</v>
+        <v>0.09041274734203091</v>
       </c>
     </row>
     <row r="170">
@@ -2306,7 +2306,7 @@
         <v>0.2976190476190476</v>
       </c>
       <c r="C170" t="n">
-        <v>0.05077988055154205</v>
+        <v>0.08943283566059028</v>
       </c>
     </row>
     <row r="171">
@@ -2317,7 +2317,7 @@
         <v>0.2958579881656805</v>
       </c>
       <c r="C171" t="n">
-        <v>0.05016154540923769</v>
+        <v>0.08847233243951688</v>
       </c>
     </row>
     <row r="172">
@@ -2328,7 +2328,7 @@
         <v>0.2941176470588235</v>
       </c>
       <c r="C172" t="n">
-        <v>0.04959028951496024</v>
+        <v>0.08752948308315932</v>
       </c>
     </row>
     <row r="173">
@@ -2339,7 +2339,7 @@
         <v>0.2923976608187134</v>
       </c>
       <c r="C173" t="n">
-        <v>0.04905827324750296</v>
+        <v>0.08660281737148248</v>
       </c>
     </row>
     <row r="174">
@@ -2350,7 +2350,7 @@
         <v>0.2906976744186047</v>
       </c>
       <c r="C174" t="n">
-        <v>0.04854158629520631</v>
+        <v>0.08569195263895051</v>
       </c>
     </row>
     <row r="175">
@@ -2361,7 +2361,7 @@
         <v>0.2890173410404624</v>
       </c>
       <c r="C175" t="n">
-        <v>0.04803256698945935</v>
+        <v>0.0847965177812683</v>
       </c>
     </row>
     <row r="176">
@@ -2372,7 +2372,7 @@
         <v>0.2873563218390804</v>
       </c>
       <c r="C176" t="n">
-        <v>0.04753114733945087</v>
+        <v>0.0839161530017976</v>
       </c>
     </row>
     <row r="177">
@@ -2383,7 +2383,7 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="C177" t="n">
-        <v>0.04703725598672113</v>
+        <v>0.08305050953195528</v>
       </c>
     </row>
     <row r="178">
@@ -2394,7 +2394,7 @@
         <v>0.2840909090909091</v>
       </c>
       <c r="C178" t="n">
-        <v>0.04655081846249478</v>
+        <v>0.08219924934353466</v>
       </c>
     </row>
     <row r="179">
@@ -2405,7 +2405,7 @@
         <v>0.2824858757062147</v>
       </c>
       <c r="C179" t="n">
-        <v>0.0460717574387967</v>
+        <v>0.08136204484908385</v>
       </c>
     </row>
     <row r="180">
@@ -2416,7 +2416,7 @@
         <v>0.2808988764044944</v>
       </c>
       <c r="C180" t="n">
-        <v>0.04560151986454899</v>
+        <v>0.08054071624194255</v>
       </c>
     </row>
     <row r="181">
@@ -2427,7 +2427,7 @@
         <v>0.2793296089385475</v>
       </c>
       <c r="C181" t="n">
-        <v>0.04513933637608732</v>
+        <v>0.07973594187628077</v>
       </c>
     </row>
     <row r="182">
@@ -2438,7 +2438,7 @@
         <v>0.2777777777777778</v>
       </c>
       <c r="C182" t="n">
-        <v>0.04468423120176099</v>
+        <v>0.07894556593799235</v>
       </c>
     </row>
     <row r="183">
@@ -2449,7 +2449,7 @@
         <v>0.2762430939226519</v>
       </c>
       <c r="C183" t="n">
-        <v>0.04423611913776015</v>
+        <v>0.07816789283756813</v>
       </c>
     </row>
     <row r="184">
@@ -2460,7 +2460,7 @@
         <v>0.2747252747252747</v>
       </c>
       <c r="C184" t="n">
-        <v>0.04379491323244353</v>
+        <v>0.07740264582602502</v>
       </c>
     </row>
     <row r="185">
@@ -2471,7 +2471,7 @@
         <v>0.273224043715847</v>
       </c>
       <c r="C185" t="n">
-        <v>0.04336052499207612</v>
+        <v>0.07664955662605573</v>
       </c>
     </row>
     <row r="186">
@@ -2482,7 +2482,7 @@
         <v>0.2717391304347826</v>
       </c>
       <c r="C186" t="n">
-        <v>0.04293367880443896</v>
+        <v>0.07590950504531681</v>
       </c>
     </row>
     <row r="187">
@@ -2493,7 +2493,7 @@
         <v>0.2702702702702702</v>
       </c>
       <c r="C187" t="n">
-        <v>0.04251485702272732</v>
+        <v>0.07518304153152534</v>
       </c>
     </row>
     <row r="188">
@@ -2504,7 +2504,7 @@
         <v>0.2688172043010753</v>
       </c>
       <c r="C188" t="n">
-        <v>0.04210253497673706</v>
+        <v>0.07446791564684352</v>
       </c>
     </row>
     <row r="189">
@@ -2515,7 +2515,7 @@
         <v>0.267379679144385</v>
       </c>
       <c r="C189" t="n">
-        <v>0.04169662089388966</v>
+        <v>0.07376389143214786</v>
       </c>
     </row>
     <row r="190">
@@ -2526,7 +2526,7 @@
         <v>0.2659574468085106</v>
       </c>
       <c r="C190" t="n">
-        <v>0.04129762481328674</v>
+        <v>0.07307158338254816</v>
       </c>
     </row>
     <row r="191">
@@ -2537,7 +2537,7 @@
         <v>0.2645502645502645</v>
       </c>
       <c r="C191" t="n">
-        <v>0.04090607916875688</v>
+        <v>0.07239164477944904</v>
       </c>
     </row>
     <row r="192">
@@ -2548,7 +2548,7 @@
         <v>0.2631578947368421</v>
       </c>
       <c r="C192" t="n">
-        <v>0.04052062357458828</v>
+        <v>0.07172208592655487</v>
       </c>
     </row>
     <row r="193">
@@ -2559,7 +2559,7 @@
         <v>0.2617801047120419</v>
       </c>
       <c r="C193" t="n">
-        <v>0.04014116535990445</v>
+        <v>0.07106269845307588</v>
       </c>
     </row>
     <row r="194">
@@ -2570,7 +2570,7 @@
         <v>0.2604166666666667</v>
       </c>
       <c r="C194" t="n">
-        <v>0.03976761168356437</v>
+        <v>0.07041327985207566</v>
       </c>
     </row>
     <row r="195">
@@ -2581,7 +2581,7 @@
         <v>0.2590673575129534</v>
       </c>
       <c r="C195" t="n">
-        <v>0.03939986965417181</v>
+        <v>0.0697736332426384</v>
       </c>
     </row>
     <row r="196">
@@ -2592,7 +2592,7 @@
         <v>0.2577319587628866</v>
       </c>
       <c r="C196" t="n">
-        <v>0.03903784643797541</v>
+        <v>0.06914356713787946</v>
       </c>
     </row>
     <row r="197">
@@ -2603,7 +2603,7 @@
         <v>0.2564102564102564</v>
       </c>
       <c r="C197" t="n">
-        <v>0.03868144936357713</v>
+        <v>0.06852289522516025</v>
       </c>
     </row>
     <row r="198">
@@ -2614,7 +2614,7 @@
         <v>0.2551020408163265</v>
       </c>
       <c r="C198" t="n">
-        <v>0.03833058601907344</v>
+        <v>0.06791143615673399</v>
       </c>
     </row>
     <row r="199">
@@ -2625,7 +2625,7 @@
         <v>0.2538071065989848</v>
       </c>
       <c r="C199" t="n">
-        <v>0.03798516434041692</v>
+        <v>0.06730901334314829</v>
       </c>
     </row>
     <row r="200">
@@ -2636,7 +2636,7 @@
         <v>0.2525252525252525</v>
       </c>
       <c r="C200" t="n">
-        <v>0.03764509269464502</v>
+        <v>0.06671545476266623</v>
       </c>
     </row>
     <row r="201">
@@ -2647,7 +2647,7 @@
         <v>0.2512562814070352</v>
       </c>
       <c r="C201" t="n">
-        <v>0.03736651944664506</v>
+        <v>0.06620932805857421</v>
       </c>
     </row>
     <row r="202">
@@ -2658,7 +2658,7 @@
         <v>0.25</v>
       </c>
       <c r="C202" t="n">
-        <v>0.03713197852348136</v>
+        <v>0.06576614405411818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>